<commit_message>
Haven't quite nailed this down yet
</commit_message>
<xml_diff>
--- a/IO_M2.1_new/MattC_RunControl_initRuns.xlsx
+++ b/IO_M2.1_new/MattC_RunControl_initRuns.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" state="visible" r:id="rId2"/>
@@ -2303,9 +2303,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>606240</xdr:colOff>
+      <xdr:colOff>605880</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2314,8 +2314,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8213760" y="3313440"/>
-          <a:ext cx="2526840" cy="1531080"/>
+          <a:off x="8242200" y="3313440"/>
+          <a:ext cx="2526840" cy="1530720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2742,7 +2742,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2807,22 +2807,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3825,7 +3825,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.1376518218623"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="27" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="27" width="11.6761133603239"/>
@@ -4538,26 +4538,26 @@
   </sheetPr>
   <dimension ref="A1:AY110"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topRight" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.8056680161943"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.3441295546559"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="true" max="10" min="9" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="16" min="15" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="21" min="17" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.3886639676113"/>
@@ -4567,7 +4567,7 @@
     <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="4" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="36" min="32" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="41" min="38" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="43" min="42" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="48" min="44" style="0" width="13.3886639676113"/>
@@ -18668,13 +18668,13 @@
   </sheetPr>
   <dimension ref="A3:D6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -18694,7 +18694,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.075</v>
@@ -18706,9 +18706,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>0.025</v>
@@ -18720,9 +18720,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>0.075</v>
@@ -18794,7 +18794,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18850,7 +18850,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -18877,9 +18877,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.03643724696356"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="93.2995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.1578947368421"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -19297,12 +19297,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="120.080971659919"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="121.14979757085"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="62.9878542510121"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.5222672064777"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -19961,11 +19961,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4210526315789"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.4493927125506"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="78.8380566801619"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.9878542510121"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.5910931174089"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>